<commit_message>
Updated FIN_grids model - 2025-08-26 02:23
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_FIN_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FIN_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D306DD3C-F4EA-4896-93CF-0469A6E28936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0995DA6E-DDA8-4DE2-BA07-5CA1B76449BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4348,7 +4348,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58A400E4-4FB8-3B21-F42A-5502C2FAE2A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D47F4C-758F-A97A-B76F-ABCF99571969}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4403,7 +4403,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4011E6D6-F236-4629-E764-4834914C2F24}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68B8D43A-4E32-C586-4589-253603B4E724}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4458,7 +4458,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4284C05C-AA8B-CA8D-174F-85AC580A69C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{531C861D-B4FB-5A87-37D1-2F8F12749137}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4513,7 +4513,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFEA217-0A31-F03E-BA8D-27691A6258D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64CDD225-61B2-AF99-1A9D-9672E230F0BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4568,7 +4568,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC3FB144-6CA5-18B0-BA50-58E179FC2510}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C75628-524C-EF74-0879-8B5257A79BE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8498,7 +8498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A32EC11-2C02-483E-866F-4B0DCDB038D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A22F740-80C1-4039-A2FB-A91A73F30040}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8722,7 +8722,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B044BDDF-7162-4479-96CC-A8A3F95C2E99}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92755653-8B68-4B09-A28E-CA4A528CC7D9}">
   <dimension ref="A1:O205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16488,7 +16488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8C976F-D174-43A8-B95A-50458EEC3AF1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E34700-8841-405E-BC6A-41AEAF8149D8}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18354,7 +18354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD91230C-20F7-42F5-A03C-7838FB4DBE51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF3DFB0-E65B-4513-AD63-02ABEA8694A0}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated FIN_grids model - 2025-08-26 14:33
</commit_message>
<xml_diff>
--- a/VerveStacks_FIN_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_FIN_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_FIN_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0995DA6E-DDA8-4DE2-BA07-5CA1B76449BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{139681C8-B706-4A8E-A86B-DE9AA30EB392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4348,7 +4348,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D47F4C-758F-A97A-B76F-ABCF99571969}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D5EC61-EDDE-ED1A-1251-A577F7A3C6B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4403,7 +4403,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68B8D43A-4E32-C586-4589-253603B4E724}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06FAA0D1-360A-DF0A-9812-C54FFCF4F468}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4458,7 +4458,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{531C861D-B4FB-5A87-37D1-2F8F12749137}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43DE8002-3422-B08F-2D05-E110670CF664}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4513,7 +4513,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64CDD225-61B2-AF99-1A9D-9672E230F0BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7286689-1560-9A54-3736-E898CD9E69EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4568,7 +4568,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C75628-524C-EF74-0879-8B5257A79BE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C770B247-2DC9-095A-E020-7796C2EB28E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8498,7 +8498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A22F740-80C1-4039-A2FB-A91A73F30040}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9CCEC7-EA12-42DF-BA91-4A92CCB5C993}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8722,7 +8722,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92755653-8B68-4B09-A28E-CA4A528CC7D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9002D627-EF72-4DB3-8E20-1A2F5544455C}">
   <dimension ref="A1:O205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16488,7 +16488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E34700-8841-405E-BC6A-41AEAF8149D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A4B709-F6CB-4A4D-99C6-0F8711BEAA34}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18354,7 +18354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF3DFB0-E65B-4513-AD63-02ABEA8694A0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1498E438-727B-4368-B260-278D61A4A441}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>